<commit_message>
Conexión del gestor de géneros
- Corregir unos estilos de formularios
- Crear todas la sconexiones que consumiran los controladores para agrefar y eliminar
</commit_message>
<xml_diff>
--- a/temp/Reservaciones.xlsx
+++ b/temp/Reservaciones.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -26,7 +26,7 @@
     <t>CELULAR</t>
   </si>
   <si>
-    <t>DEPOSITO REALZADO</t>
+    <t>DEPÓSITO REALZADO</t>
   </si>
   <si>
     <t>NO. PERSONAS</t>
@@ -47,61 +47,127 @@
     <t>NO. MESA</t>
   </si>
   <si>
-    <t>victor</t>
+    <t>Itzel</t>
+  </si>
+  <si>
+    <t>aumi@hotmail.com</t>
+  </si>
+  <si>
+    <t>5578529876</t>
+  </si>
+  <si>
+    <t>No aplica</t>
+  </si>
+  <si>
+    <t>Abel Mireles Cuarteto</t>
+  </si>
+  <si>
+    <t>$150.00</t>
+  </si>
+  <si>
+    <t>26-03-2019</t>
+  </si>
+  <si>
+    <t>22:30</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>anto@gmail.com</t>
+  </si>
+  <si>
+    <t>5632659841</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Juan@gmail.com</t>
+  </si>
+  <si>
+    <t>5512356984</t>
+  </si>
+  <si>
+    <t>Pablo</t>
+  </si>
+  <si>
+    <t>pablo@gmail.com</t>
+  </si>
+  <si>
+    <t>5554896325</t>
+  </si>
+  <si>
+    <t>Sala Jack 2</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>luis@gmail.com</t>
+  </si>
+  <si>
+    <t>5698741236</t>
+  </si>
+  <si>
+    <t>Victor</t>
   </si>
   <si>
     <t>victor@gmail.com</t>
   </si>
   <si>
-    <t>No aplica</t>
-  </si>
-  <si>
-    <t>Abel</t>
-  </si>
-  <si>
-    <t>$150.00</t>
-  </si>
-  <si>
-    <t>27-04-2019</t>
-  </si>
-  <si>
-    <t>01:08</t>
-  </si>
-  <si>
-    <t>Sala Jack 1</t>
-  </si>
-  <si>
-    <t>Cindy</t>
-  </si>
-  <si>
-    <t>cindy@gmail.com</t>
-  </si>
-  <si>
-    <t>Deposito realizado</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>$200.00</t>
-  </si>
-  <si>
-    <t>03-05-2019</t>
-  </si>
-  <si>
-    <t>18:08</t>
-  </si>
-  <si>
-    <t>Paco</t>
-  </si>
-  <si>
-    <t>paco@gmail.com</t>
-  </si>
-  <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
-    <t>Sala Jack 3</t>
+    <t>Lupita</t>
+  </si>
+  <si>
+    <t>lupita@gmail.com</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>amilkhael@gmail.c</t>
+  </si>
+  <si>
+    <t>5540576841</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>amilkhael@gmail.com</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>Los Peseros</t>
+  </si>
+  <si>
+    <t>$0.00</t>
+  </si>
+  <si>
+    <t>16-04-2019</t>
+  </si>
+  <si>
+    <t>21:30</t>
+  </si>
+  <si>
+    <t>Eduardo Chávez Delgado</t>
+  </si>
+  <si>
+    <t>Homenaje a Johnny Cash por Cuervos Rockabilly Trío</t>
+  </si>
+  <si>
+    <t>17-04-2019</t>
+  </si>
+  <si>
+    <t>22:00</t>
+  </si>
+  <si>
+    <t>Chávez Delgado</t>
   </si>
 </sst>
 </file>
@@ -458,7 +524,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,29 +571,29 @@
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
-        <v>8787654567</v>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
+        <v>17</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -537,61 +603,635 @@
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3">
-        <v>878787878</v>
+      <c r="C3" t="s">
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="C4">
-        <v>987898757</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
         <v>27</v>
       </c>
-      <c r="E4">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11"/>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13">
+        <v>1512451215</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>28</v>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>